<commit_message>
Punteos Actividades 1 y 2
Se subio el punteo de las primeras dos actividades grupales.
</commit_message>
<xml_diff>
--- a/control de tareas Unidad II - Diego.xlsx
+++ b/control de tareas Unidad II - Diego.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdalbertoPc\Documents\luterano 2016\Bachillerato\tareas\videosDigital\PunteosActividades5to\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creacion de canal de Youtube" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +66,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +91,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +116,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -265,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -767,7 +772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,16 +782,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -836,7 +841,9 @@
       <c r="D7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -849,7 +856,9 @@
       <c r="D8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -862,7 +871,9 @@
       <c r="D9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -875,7 +886,9 @@
       <c r="D10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -888,7 +901,9 @@
       <c r="D11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -918,7 +933,7 @@
       <c r="E14" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B7:B14"/>
@@ -933,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1015,9 @@
       <c r="D7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1013,7 +1030,9 @@
       <c r="D8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1026,7 +1045,9 @@
       <c r="D9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1039,7 +1060,9 @@
       <c r="D10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1052,7 +1075,9 @@
       <c r="D11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1082,7 +1107,7 @@
       <c r="E14" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B7:B14"/>

</xml_diff>